<commit_message>
TestCase per accreditamento EDINEXT SRL
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EDINEXTSRL/EDINEXT_SRL/AVR/v2.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111EDINEXTSRL/EDINEXT_SRL/AVR/v2.0.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\OneDrive\Desktop\fse2\TENTATIVO3\scheda_vaccinale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\OneDrive\Desktop\fse2\4_invio_completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C1E145-F8A1-4328-B6D5-161FC30BCB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72FFA5A-C53F-466F-9FCD-22112BCC9CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="390" windowWidth="28800" windowHeight="15150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="262">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1548,7 +1548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1671,6 +1671,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1711,63 +1732,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3216,10 +3180,10 @@
   <dimension ref="A1:T876"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38:XFD38"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3265,14 +3229,14 @@
       <c r="T1" s="20"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="45" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -3290,14 +3254,14 @@
       <c r="T2" s="20"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="52" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="44"/>
+      <c r="D3" s="50"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -3315,12 +3279,12 @@
       <c r="T3" s="20"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="52" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="D4" s="44"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="22"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
@@ -3339,12 +3303,12 @@
       <c r="T4" s="20"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="44"/>
+      <c r="D5" s="50"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -3362,8 +3326,8 @@
       <c r="T5" s="20"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="23"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -3710,7 +3674,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27">
         <v>42</v>
       </c>
@@ -3762,53 +3726,55 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="65" customFormat="1" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="56">
+    <row r="16" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27">
         <v>50</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="66">
+      <c r="F16" s="44">
         <v>44972</v>
       </c>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="61" t="s">
+      <c r="G16" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="K16" s="61" t="s">
+      <c r="K16" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="L16" s="61" t="s">
+      <c r="L16" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="M16" s="61" t="s">
+      <c r="M16" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61" t="s">
+      <c r="N16" s="30"/>
+      <c r="O16" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="P16" s="68" t="s">
+      <c r="P16" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="Q16" s="61"/>
-      <c r="R16" s="62" t="s">
+      <c r="Q16" s="30"/>
+      <c r="R16" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="S16" s="63"/>
-      <c r="T16" s="64" t="s">
+      <c r="S16" s="31"/>
+      <c r="T16" s="35" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4638,19 +4604,21 @@
       <c r="E32" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="F32" s="53">
+      <c r="F32" s="41">
         <v>44974</v>
       </c>
-      <c r="G32" s="54" t="s">
+      <c r="G32" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="H32" s="54" t="s">
+      <c r="H32" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="I32" s="54" t="s">
+      <c r="I32" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="J32" s="30"/>
+      <c r="J32" s="30" t="s">
+        <v>35</v>
+      </c>
       <c r="K32" s="30"/>
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
@@ -4680,19 +4648,21 @@
       <c r="E33" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="F33" s="53">
+      <c r="F33" s="41">
         <v>44974</v>
       </c>
-      <c r="G33" s="54" t="s">
+      <c r="G33" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="H33" s="54" t="s">
+      <c r="H33" s="42" t="s">
         <v>240</v>
       </c>
-      <c r="I33" s="54" t="s">
+      <c r="I33" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="J33" s="30"/>
+      <c r="J33" s="30" t="s">
+        <v>35</v>
+      </c>
       <c r="K33" s="30"/>
       <c r="L33" s="30"/>
       <c r="M33" s="30"/>
@@ -4722,16 +4692,16 @@
       <c r="E34" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="53">
+      <c r="F34" s="41">
         <v>44974</v>
       </c>
-      <c r="G34" s="54" t="s">
+      <c r="G34" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="H34" s="54" t="s">
+      <c r="H34" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="I34" s="54" t="s">
+      <c r="I34" s="42" t="s">
         <v>245</v>
       </c>
       <c r="J34" s="30" t="s">
@@ -4766,16 +4736,16 @@
       <c r="E35" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="F35" s="53">
+      <c r="F35" s="41">
         <v>44974</v>
       </c>
-      <c r="G35" s="54" t="s">
+      <c r="G35" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="H35" s="54" t="s">
+      <c r="H35" s="42" t="s">
         <v>242</v>
       </c>
-      <c r="I35" s="54" t="s">
+      <c r="I35" s="42" t="s">
         <v>246</v>
       </c>
       <c r="J35" s="30" t="s">
@@ -4794,36 +4764,36 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="65" customFormat="1" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="56">
+    <row r="36" spans="1:20" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27">
         <v>33</v>
       </c>
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="53">
+      <c r="F36" s="41">
         <v>44974</v>
       </c>
-      <c r="G36" s="60" t="s">
+      <c r="G36" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="H36" s="60" t="s">
+      <c r="H36" s="42" t="s">
         <v>224</v>
       </c>
-      <c r="I36" s="60"/>
-      <c r="J36" s="61" t="s">
+      <c r="I36" s="42"/>
+      <c r="J36" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="K36" s="61"/>
+      <c r="K36" s="30"/>
       <c r="L36" s="30" t="s">
         <v>79</v>
       </c>
@@ -4837,16 +4807,16 @@
       <c r="P36" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="Q36" s="61"/>
-      <c r="R36" s="62"/>
-      <c r="S36" s="63" t="s">
+      <c r="Q36" s="30"/>
+      <c r="R36" s="33"/>
+      <c r="S36" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="T36" s="64" t="s">
+      <c r="T36" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27">
         <v>41</v>
       </c>
@@ -4862,16 +4832,16 @@
       <c r="E37" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="53">
+      <c r="F37" s="41">
         <v>44974</v>
       </c>
-      <c r="G37" s="54" t="s">
+      <c r="G37" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="H37" s="54" t="s">
+      <c r="H37" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="I37" s="54"/>
+      <c r="I37" s="42"/>
       <c r="J37" s="30" t="s">
         <v>35</v>
       </c>
@@ -4898,43 +4868,55 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:20" s="65" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="56">
+    <row r="38" spans="1:20" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27">
         <v>49</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="57" t="s">
+      <c r="C38" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="57" t="s">
+      <c r="D38" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="E38" s="58" t="s">
+      <c r="E38" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="59"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="61" t="s">
+      <c r="F38" s="41">
+        <v>44972</v>
+      </c>
+      <c r="G38" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="K38" s="61" t="s">
+      <c r="K38" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="61"/>
-      <c r="O38" s="61"/>
-      <c r="P38" s="61"/>
-      <c r="Q38" s="61"/>
-      <c r="R38" s="62" t="s">
+      <c r="L38" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="M38" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="N38" s="30"/>
+      <c r="O38" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="S38" s="63"/>
-      <c r="T38" s="64" t="s">
+      <c r="P38" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="S38" s="31"/>
+      <c r="T38" s="35" t="s">
         <v>88</v>
       </c>
     </row>
@@ -4954,16 +4936,16 @@
       <c r="E39" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="F39" s="53">
+      <c r="F39" s="41">
         <v>44974</v>
       </c>
-      <c r="G39" s="54" t="s">
+      <c r="G39" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="H39" s="54" t="s">
+      <c r="H39" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="I39" s="54" t="s">
+      <c r="I39" s="42" t="s">
         <v>247</v>
       </c>
       <c r="J39" s="30" t="s">
@@ -5008,16 +4990,16 @@
       <c r="E40" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="F40" s="53">
+      <c r="F40" s="41">
         <v>44974</v>
       </c>
-      <c r="G40" s="54" t="s">
+      <c r="G40" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="H40" s="54" t="s">
+      <c r="H40" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="I40" s="54" t="s">
+      <c r="I40" s="42" t="s">
         <v>248</v>
       </c>
       <c r="J40" s="30" t="s">
@@ -5062,16 +5044,16 @@
       <c r="E41" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="F41" s="53">
+      <c r="F41" s="41">
         <v>44974</v>
       </c>
-      <c r="G41" s="54" t="s">
+      <c r="G41" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="H41" s="54" t="s">
+      <c r="H41" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="I41" s="54" t="s">
+      <c r="I41" s="42" t="s">
         <v>249</v>
       </c>
       <c r="J41" s="30" t="s">
@@ -5100,7 +5082,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27">
         <v>97</v>
       </c>
@@ -5116,16 +5098,16 @@
       <c r="E42" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="F42" s="53">
+      <c r="F42" s="41">
         <v>44974</v>
       </c>
-      <c r="G42" s="54" t="s">
+      <c r="G42" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="H42" s="54" t="s">
+      <c r="H42" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I42" s="54" t="s">
+      <c r="I42" s="42" t="s">
         <v>250</v>
       </c>
       <c r="J42" s="30" t="s">
@@ -5154,7 +5136,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27">
         <v>98</v>
       </c>
@@ -5170,27 +5152,35 @@
       <c r="E43" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="F43" s="53">
+      <c r="F43" s="41">
         <v>44974</v>
       </c>
-      <c r="G43" s="54" t="s">
+      <c r="G43" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="I43" s="54" t="s">
+      <c r="I43" s="42" t="s">
         <v>251</v>
       </c>
       <c r="J43" s="30" t="s">
         <v>35</v>
       </c>
       <c r="K43" s="30"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="30"/>
+      <c r="L43" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="M43" s="30" t="s">
+        <v>79</v>
+      </c>
       <c r="N43" s="30"/>
-      <c r="O43" s="30"/>
-      <c r="P43" s="30"/>
+      <c r="O43" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="P43" s="30" t="s">
+        <v>159</v>
+      </c>
       <c r="Q43" s="30"/>
       <c r="R43" s="33"/>
       <c r="S43" s="31" t="s">
@@ -5200,7 +5190,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27">
         <v>99</v>
       </c>
@@ -5216,16 +5206,16 @@
       <c r="E44" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="F44" s="53">
+      <c r="F44" s="41">
         <v>44974</v>
       </c>
-      <c r="G44" s="54" t="s">
+      <c r="G44" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="H44" s="54" t="s">
+      <c r="H44" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="I44" s="54" t="s">
+      <c r="I44" s="42" t="s">
         <v>252</v>
       </c>
       <c r="J44" s="30" t="s">
@@ -5270,16 +5260,16 @@
       <c r="E45" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="F45" s="53">
+      <c r="F45" s="41">
         <v>44974</v>
       </c>
-      <c r="G45" s="54" t="s">
+      <c r="G45" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="H45" s="54" t="s">
+      <c r="H45" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="I45" s="54" t="s">
+      <c r="I45" s="42" t="s">
         <v>253</v>
       </c>
       <c r="J45" s="30" t="s">
@@ -5324,16 +5314,16 @@
       <c r="E46" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="F46" s="53">
+      <c r="F46" s="41">
         <v>44974</v>
       </c>
-      <c r="G46" s="54" t="s">
+      <c r="G46" s="42" t="s">
         <v>218</v>
       </c>
-      <c r="H46" s="54" t="s">
+      <c r="H46" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="I46" s="54" t="s">
+      <c r="I46" s="42" t="s">
         <v>254</v>
       </c>
       <c r="J46" s="30" t="s">
@@ -5378,16 +5368,16 @@
       <c r="E47" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="F47" s="53">
+      <c r="F47" s="41">
         <v>44974</v>
       </c>
-      <c r="G47" s="54" t="s">
+      <c r="G47" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="H47" s="54" t="s">
+      <c r="H47" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="I47" s="54" t="s">
+      <c r="I47" s="42" t="s">
         <v>255</v>
       </c>
       <c r="J47" s="30" t="s">
@@ -5432,16 +5422,16 @@
       <c r="E48" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="F48" s="53">
+      <c r="F48" s="41">
         <v>44974</v>
       </c>
-      <c r="G48" s="54" t="s">
+      <c r="G48" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="H48" s="54" t="s">
+      <c r="H48" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="I48" s="54" t="s">
+      <c r="I48" s="42" t="s">
         <v>256</v>
       </c>
       <c r="J48" s="30" t="s">
@@ -5486,16 +5476,16 @@
       <c r="E49" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="F49" s="53">
+      <c r="F49" s="41">
         <v>44974</v>
       </c>
-      <c r="G49" s="54" t="s">
+      <c r="G49" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="H49" s="55" t="s">
+      <c r="H49" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="I49" s="54" t="s">
+      <c r="I49" s="42" t="s">
         <v>257</v>
       </c>
       <c r="J49" s="30" t="s">
@@ -5540,16 +5530,16 @@
       <c r="E50" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="F50" s="53">
+      <c r="F50" s="41">
         <v>44974</v>
       </c>
-      <c r="G50" s="54" t="s">
+      <c r="G50" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="H50" s="54" t="s">
+      <c r="H50" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="I50" s="54" t="s">
+      <c r="I50" s="42" t="s">
         <v>258</v>
       </c>
       <c r="J50" s="30" t="s">
@@ -5578,7 +5568,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="270" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <v>106</v>
       </c>
@@ -5594,16 +5584,16 @@
       <c r="E51" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="F51" s="53">
+      <c r="F51" s="41">
         <v>44974</v>
       </c>
-      <c r="G51" s="54" t="s">
+      <c r="G51" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="H51" s="54" t="s">
+      <c r="H51" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="I51" s="54" t="s">
+      <c r="I51" s="42" t="s">
         <v>259</v>
       </c>
       <c r="J51" s="30" t="s">
@@ -21802,26 +21792,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -22052,32 +22022,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22096,6 +22061,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>